<commit_message>
Nuevo archivo de ejemplo de SQL injection
</commit_message>
<xml_diff>
--- a/public/informes/otro_nombre.xlsx
+++ b/public/informes/otro_nombre.xlsx
@@ -10,73 +10,28 @@
     <sheet name="Mi hoja guay" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mi hoja guay'!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mi hoja guay'!$A$3:$B$3</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>Informe dispersión 18-07-2018</t>
+    <t>Informe de Actividad 16-11-2018</t>
   </si>
   <si>
-    <t>id_cliente</t>
+    <t>matricula</t>
   </si>
   <si>
     <t>nombre</t>
   </si>
   <si>
-    <t>Documento</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>MACAULAY CULKIN</t>
-  </si>
-  <si>
-    <t>3435K</t>
-  </si>
-  <si>
-    <t>SOLOENCASA@SI.COM</t>
-  </si>
-  <si>
-    <t>ALFONSO RIBEIRO</t>
-  </si>
-  <si>
-    <t>1323E</t>
-  </si>
-  <si>
-    <t>CARACARTON@SI.COM</t>
-  </si>
-  <si>
-    <t>DAVID HASSELHOFF</t>
-  </si>
-  <si>
-    <t>6567A</t>
-  </si>
-  <si>
-    <t>MITCHBUCANAN@SI.COM</t>
-  </si>
-  <si>
     <t>MARIE CURIE</t>
   </si>
   <si>
-    <t>4356B</t>
-  </si>
-  <si>
-    <t>BRILLOENLAOSCURIDAD@SI.COM</t>
-  </si>
-  <si>
     <t>JOHNNY 5</t>
-  </si>
-  <si>
-    <t>3141P</t>
-  </si>
-  <si>
-    <t>CORTOCIRCUITO@SI.COM</t>
   </si>
 </sst>
 </file>
@@ -444,121 +399,57 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="true" style="0"/>
-    <col min="2" max="2" width="19.995117" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="11.711426" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:2">
       <c r="A2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <autoFilter ref="A3:D3"/>
+  <autoFilter ref="A3:B3"/>
   <mergeCells>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>